<commit_message>
nf 12 oct 2021 10:27PM
</commit_message>
<xml_diff>
--- a/document-test.xlsx
+++ b/document-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61011\Desktop\mini-plant-app\mini-plant-service-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900063F2-DEB2-4710-9BFD-ABE76DD193D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4AE6B0-D9D0-4DAC-8036-BD88AC0533EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="6390" windowWidth="20730" windowHeight="11310" xr2:uid="{0516D730-BA96-42EA-9942-EA5C8FA89769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="59">
   <si>
     <t>Functions</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>./shop/rate/edit</t>
+  </si>
+  <si>
+    <t>./promotion/related_to_product/add</t>
+  </si>
+  <si>
+    <t>./promotion/related_to_product/remove</t>
   </si>
 </sst>
 </file>
@@ -544,6 +550,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -557,38 +595,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DE177A-7FEF-48EA-B8AD-276CB4A222C6}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -915,7 +921,7 @@
     <col min="1" max="1" width="4.25" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="9.75" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="9.75" customWidth="1"/>
@@ -926,35 +932,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="47" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="47" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="22" t="s">
         <v>52</v>
       </c>
@@ -986,10 +992,10 @@
       <c r="B3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24" t="s">
         <v>4</v>
@@ -1018,10 +1024,10 @@
       <c r="B4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
@@ -1048,10 +1054,10 @@
       <c r="B5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
@@ -1078,10 +1084,10 @@
       <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23" t="s">
         <v>4</v>
@@ -1110,10 +1116,10 @@
       <c r="B7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="23" t="s">
         <v>4</v>
       </c>
@@ -1140,10 +1146,10 @@
       <c r="B8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="23" t="s">
         <v>4</v>
       </c>
@@ -1170,10 +1176,10 @@
       <c r="B9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="23" t="s">
         <v>4</v>
       </c>
@@ -1200,10 +1206,10 @@
       <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23" t="s">
         <v>4</v>
@@ -1232,10 +1238,10 @@
       <c r="B11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="23" t="s">
         <v>4</v>
       </c>
@@ -1266,10 +1272,10 @@
       <c r="B12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
@@ -1296,10 +1302,10 @@
       <c r="B13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23" t="s">
         <v>4</v>
@@ -1328,10 +1334,10 @@
       <c r="B14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="23" t="s">
         <v>4</v>
       </c>
@@ -1358,10 +1364,10 @@
       <c r="B15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="49"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
         <v>4</v>
@@ -1390,10 +1396,10 @@
       <c r="B16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="23" t="s">
         <v>4</v>
       </c>
@@ -1420,10 +1426,10 @@
       <c r="B17" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23" t="s">
         <v>4</v>
@@ -1452,10 +1458,10 @@
       <c r="B18" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="23" t="s">
         <v>4</v>
       </c>
@@ -1484,10 +1490,10 @@
       <c r="B19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="39"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="23" t="s">
         <v>4</v>
       </c>
@@ -1516,10 +1522,10 @@
       <c r="B20" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="39"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="23" t="s">
         <v>4</v>
       </c>
@@ -1548,10 +1554,10 @@
       <c r="B21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="39"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="23"/>
       <c r="F21" s="23" t="s">
         <v>4</v>
@@ -1580,10 +1586,10 @@
       <c r="B22" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="39"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="23" t="s">
         <v>4</v>
       </c>
@@ -1610,10 +1616,10 @@
       <c r="B23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="23" t="s">
         <v>4</v>
       </c>
@@ -1640,10 +1646,10 @@
       <c r="B24" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="23" t="s">
         <v>4</v>
       </c>
@@ -1672,10 +1678,10 @@
       <c r="B25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="39"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="23" t="s">
         <v>4</v>
       </c>
@@ -1702,10 +1708,10 @@
       <c r="B26" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="41"/>
+      <c r="D26" s="36"/>
       <c r="E26" s="23" t="s">
         <v>4</v>
       </c>
@@ -1734,10 +1740,10 @@
       <c r="B27" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="36"/>
       <c r="E27" s="23" t="s">
         <v>4</v>
       </c>
@@ -1764,10 +1770,10 @@
       <c r="B28" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="41"/>
+      <c r="D28" s="36"/>
       <c r="E28" s="23" t="s">
         <v>4</v>
       </c>
@@ -1794,10 +1800,10 @@
       <c r="B29" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="23" t="s">
         <v>4</v>
       </c>
@@ -1824,10 +1830,10 @@
       <c r="B30" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="41"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="23" t="s">
         <v>4</v>
       </c>
@@ -1854,10 +1860,10 @@
       <c r="B31" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="41"/>
+      <c r="D31" s="36"/>
       <c r="E31" s="23" t="s">
         <v>4</v>
       </c>
@@ -1884,10 +1890,10 @@
       <c r="B32" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="39"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="23"/>
       <c r="F32" s="23" t="s">
         <v>4</v>
@@ -1916,10 +1922,10 @@
       <c r="B33" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="39"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="23" t="s">
         <v>4</v>
       </c>
@@ -1946,10 +1952,10 @@
       <c r="B34" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="23" t="s">
         <v>4</v>
       </c>
@@ -1974,21 +1980,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="39"/>
+        <v>14</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="49"/>
       <c r="E35" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F35" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="23" t="s">
-        <v>4</v>
-      </c>
+      <c r="G35" s="23"/>
       <c r="H35" s="25"/>
       <c r="I35" s="11" t="s">
         <v>25</v>
@@ -2006,22 +2010,20 @@
         <v>34</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G36" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" s="27" t="s">
-        <v>4</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="49"/>
+      <c r="E36" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="23"/>
+      <c r="H36" s="25"/>
       <c r="I36" s="11" t="s">
         <v>25</v>
       </c>
@@ -2038,122 +2040,161 @@
         <v>35</v>
       </c>
       <c r="B37" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="25"/>
+      <c r="I37" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="23">
+        <v>36</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="34"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="23">
+        <v>37</v>
+      </c>
+      <c r="B39" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C39" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="D39" s="34"/>
+      <c r="E39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="25"/>
+      <c r="I39" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B41" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="4" t="s">
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K41" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="30">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="30">
         <v>1</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B42" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K40" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L41" s="21"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L43" s="21"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="B40:H40"/>
+  <mergeCells count="43">
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C16:D16"/>
@@ -2164,11 +2205,38 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
banks 16 oct 2021 4:43PM
</commit_message>
<xml_diff>
--- a/document-test.xlsx
+++ b/document-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61011\Desktop\mini-plant-app\mini-plant-service-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4AE6B0-D9D0-4DAC-8036-BD88AC0533EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C10ADA-89EF-4CF3-9572-83D3BD1F999C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="6390" windowWidth="20730" windowHeight="11310" xr2:uid="{0516D730-BA96-42EA-9942-EA5C8FA89769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="64">
   <si>
     <t>Functions</t>
   </si>
@@ -211,6 +211,21 @@
   </si>
   <si>
     <t>./promotion/related_to_product/remove</t>
+  </si>
+  <si>
+    <t>./shop/bank</t>
+  </si>
+  <si>
+    <t>./shop/bank/add</t>
+  </si>
+  <si>
+    <t>./shop/bank/edit</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>./shop/bank/delete</t>
   </si>
 </sst>
 </file>
@@ -557,6 +572,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,12 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DE177A-7FEF-48EA-B8AD-276CB4A222C6}">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -932,35 +947,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="37" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="37" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="22" t="s">
         <v>52</v>
       </c>
@@ -1364,10 +1379,10 @@
       <c r="B15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="49"/>
+      <c r="C15" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="38"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
         <v>4</v>
@@ -1375,7 +1390,7 @@
       <c r="G15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="23" t="s">
         <v>4</v>
       </c>
       <c r="I15" s="11" t="s">
@@ -1387,26 +1402,28 @@
       <c r="K15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="23">
         <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="34"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="38"/>
       <c r="E16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23" t="s">
-        <v>4</v>
-      </c>
+      <c r="F16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="23"/>
       <c r="H16" s="25"/>
       <c r="I16" s="11" t="s">
         <v>25</v>
@@ -1417,29 +1434,29 @@
       <c r="K16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="23">
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="23"/>
+        <v>13</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="F17" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>4</v>
-      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="11" t="s">
         <v>25</v>
       </c>
@@ -1449,29 +1466,29 @@
       <c r="K17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="23">
         <v>16</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="36"/>
+      <c r="C18" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="38"/>
       <c r="E18" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="29"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="11" t="s">
         <v>25</v>
       </c>
@@ -1481,29 +1498,31 @@
       <c r="K18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="23">
         <v>17</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="23" t="s">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="23" t="s">
         <v>4</v>
       </c>
       <c r="G19" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>4</v>
+      </c>
       <c r="I19" s="11" t="s">
         <v>25</v>
       </c>
@@ -1523,15 +1542,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="23" t="s">
-        <v>4</v>
-      </c>
+      <c r="F20" s="23"/>
       <c r="G20" s="23" t="s">
         <v>4</v>
       </c>
@@ -1555,7 +1572,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="23"/>
@@ -1583,21 +1600,23 @@
       <c r="A22" s="23">
         <v>20</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="34"/>
+      <c r="C22" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="36"/>
       <c r="E22" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F22" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="25"/>
+      <c r="G22" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="29"/>
       <c r="I22" s="11" t="s">
         <v>25</v>
       </c>
@@ -1614,10 +1633,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="23" t="s">
@@ -1626,7 +1645,9 @@
       <c r="F23" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="23"/>
+      <c r="G23" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="H23" s="25"/>
       <c r="I23" s="11" t="s">
         <v>25</v>
@@ -1644,10 +1665,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="23" t="s">
@@ -1676,20 +1697,22 @@
         <v>23</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D25" s="34"/>
-      <c r="E25" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="G25" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="25"/>
+      <c r="H25" s="25" t="s">
+        <v>4</v>
+      </c>
       <c r="I25" s="11" t="s">
         <v>25</v>
       </c>
@@ -1705,23 +1728,21 @@
       <c r="A26" s="23">
         <v>24</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="36"/>
+      <c r="B26" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="34"/>
       <c r="E26" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="31"/>
+      <c r="F26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="23"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="11" t="s">
         <v>25</v>
       </c>
@@ -1737,21 +1758,21 @@
       <c r="A27" s="23">
         <v>25</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="36"/>
+      <c r="B27" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="34"/>
       <c r="E27" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="31"/>
+      <c r="F27" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="11" t="s">
         <v>25</v>
       </c>
@@ -1767,21 +1788,23 @@
       <c r="A28" s="23">
         <v>26</v>
       </c>
-      <c r="B28" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="36"/>
+      <c r="B28" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="34"/>
       <c r="E28" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="31"/>
+      <c r="F28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="25"/>
       <c r="I28" s="11" t="s">
         <v>25</v>
       </c>
@@ -1801,17 +1824,17 @@
         <v>14</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="31"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="25"/>
       <c r="I29" s="11" t="s">
         <v>25</v>
       </c>
@@ -1828,10 +1851,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="23" t="s">
@@ -1840,8 +1863,10 @@
       <c r="F30" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="32"/>
+      <c r="G30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="31"/>
       <c r="I30" s="11" t="s">
         <v>25</v>
       </c>
@@ -1858,20 +1883,20 @@
         <v>29</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D31" s="36"/>
       <c r="E31" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="29"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="32"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="11" t="s">
         <v>25</v>
       </c>
@@ -1887,23 +1912,21 @@
       <c r="A32" s="23">
         <v>30</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>4</v>
-      </c>
+      <c r="B32" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="36"/>
+      <c r="E32" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="31"/>
       <c r="I32" s="11" t="s">
         <v>25</v>
       </c>
@@ -1923,17 +1946,17 @@
         <v>14</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D33" s="34"/>
       <c r="E33" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="25"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="31"/>
       <c r="I33" s="11" t="s">
         <v>25</v>
       </c>
@@ -1949,21 +1972,21 @@
       <c r="A34" s="23">
         <v>32</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="34"/>
+      <c r="C34" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="36"/>
       <c r="E34" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" s="23"/>
-      <c r="H34" s="25"/>
+      <c r="F34" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="29"/>
+      <c r="H34" s="32"/>
       <c r="I34" s="11" t="s">
         <v>25</v>
       </c>
@@ -1979,21 +2002,21 @@
       <c r="A35" s="23">
         <v>33</v>
       </c>
-      <c r="B35" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="49"/>
+      <c r="B35" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="36"/>
       <c r="E35" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="25"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="32"/>
       <c r="I35" s="11" t="s">
         <v>25</v>
       </c>
@@ -2010,20 +2033,22 @@
         <v>34</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" s="49"/>
-      <c r="E36" s="23" t="s">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="25"/>
+      <c r="G36" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>4</v>
+      </c>
       <c r="I36" s="11" t="s">
         <v>25</v>
       </c>
@@ -2040,10 +2065,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D37" s="34"/>
       <c r="E37" s="23" t="s">
@@ -2052,9 +2077,7 @@
       <c r="F37" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="23" t="s">
-        <v>4</v>
-      </c>
+      <c r="G37" s="23"/>
       <c r="H37" s="25"/>
       <c r="I37" s="11" t="s">
         <v>25</v>
@@ -2072,22 +2095,20 @@
         <v>36</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D38" s="34"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" s="27" t="s">
-        <v>4</v>
-      </c>
+      <c r="E38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="23"/>
+      <c r="H38" s="25"/>
       <c r="I38" s="11" t="s">
         <v>25</v>
       </c>
@@ -2106,110 +2127,234 @@
       <c r="B39" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="38"/>
+      <c r="E39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="23"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="23">
+        <v>38</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="38"/>
+      <c r="E40" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="23"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="23">
+        <v>39</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="34"/>
+      <c r="E41" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="25"/>
+      <c r="I41" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="23">
+        <v>40</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="34"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="23">
+        <v>41</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G39" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K39" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="D43" s="34"/>
+      <c r="E43" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="25"/>
+      <c r="I43" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="4" t="s">
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="30">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="30">
         <v>1</v>
       </c>
-      <c r="B42" s="45" t="s">
+      <c r="B46" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L43" s="21"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L47" s="21"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="C15:D15"/>
+  <mergeCells count="47">
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C3:D3"/>
@@ -2226,17 +2371,21 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>